<commit_message>
include label for model (started)
</commit_message>
<xml_diff>
--- a/09_Data_probands/Data_summary_children.xlsx
+++ b/09_Data_probands/Data_summary_children.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/912d11d3d824c173/Desktop/DSBA-M2/CRP/SensitivePen/09_Data_probands/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\OneDrive\Desktop\DSBA-M2\CRP\SensitivePen\09_Data_probands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{69B3C70E-D702-4616-9453-C0439ECC11AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63BF4789-0799-4801-8DEA-70B5207C799A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99031EC5-057E-457E-9368-D34BC928B112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7050" yWindow="930" windowWidth="21600" windowHeight="11295" xr2:uid="{A1CF00C3-29CF-449A-99BB-FF6FCD9F3D22}"/>
+    <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11295" xr2:uid="{A1CF00C3-29CF-449A-99BB-FF6FCD9F3D22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$E$17:$E$46</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$F$17:$F$46</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$F$17:$F$46</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$17:$E$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -640,7 +640,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -703,7 +703,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1906,7 +1906,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10525125" y="3290887"/>
+              <a:off x="9505950" y="3290887"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1984,7 +1984,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10515600" y="6196012"/>
+              <a:off x="9496425" y="6196012"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2317,8 +2317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3290B4C-D5B3-44CE-BAF9-F245E59CD938}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2376,10 +2376,9 @@
       <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2399,10 +2398,9 @@
       <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>119</v>
       </c>
-      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2422,10 +2420,9 @@
       <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2445,10 +2442,9 @@
       <c r="G5" t="s">
         <v>8</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2468,10 +2464,9 @@
       <c r="G6" t="s">
         <v>8</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2491,10 +2486,9 @@
       <c r="G7" t="s">
         <v>8</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2514,7 +2508,6 @@
       <c r="G8" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2534,10 +2527,9 @@
       <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>106</v>
       </c>
-      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -2557,10 +2549,9 @@
       <c r="G10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>107</v>
       </c>
-      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2580,10 +2571,9 @@
       <c r="G11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -2600,10 +2590,9 @@
       <c r="G12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2620,10 +2609,9 @@
       <c r="G13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>56</v>
       </c>
-      <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -2640,10 +2628,9 @@
       <c r="G14" t="s">
         <v>8</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -2663,10 +2650,9 @@
       <c r="G15" t="s">
         <v>8</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>58</v>
       </c>
-      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2686,10 +2672,9 @@
       <c r="G16" t="s">
         <v>8</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>59</v>
       </c>
-      <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -3270,10 +3255,9 @@
       <c r="G36" t="s">
         <v>8</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>73</v>
       </c>
-      <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -3293,10 +3277,9 @@
       <c r="G37" t="s">
         <v>8</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>74</v>
       </c>
-      <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -3560,10 +3543,9 @@
       <c r="G47" t="s">
         <v>8</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>83</v>
       </c>
-      <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -3580,10 +3562,9 @@
       <c r="G48" t="s">
         <v>8</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>84</v>
       </c>
-      <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">

</xml_diff>